<commit_message>
Correccion de estructura del proyecto
</commit_message>
<xml_diff>
--- a/Documentación/6. Sprint Backlog/Sprint Backlog_ver_3.xlsx
+++ b/Documentación/6. Sprint Backlog/Sprint Backlog_ver_3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29422"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\APLICACIONES\SIG-KALLARI\Documentación\6. Sprint Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B12645-0D24-4343-8207-31D81E4A2742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113D203B-67A4-4DCC-AB5C-36EC5B42E053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1146,23 +1146,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1994,8 +1994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4997E735-32F4-4641-AE3E-88C420B1F81E}">
   <dimension ref="A1:Y277"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,14 +2034,14 @@
       <c r="O1" s="28"/>
     </row>
     <row r="2" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
       <c r="H2" s="27"/>
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
@@ -2052,12 +2052,12 @@
       <c r="O2" s="28"/>
     </row>
     <row r="3" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
       <c r="H3" s="27"/>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
@@ -2068,12 +2068,12 @@
       <c r="O3" s="28"/>
     </row>
     <row r="4" spans="1:15" ht="39.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
@@ -2098,11 +2098,11 @@
       <c r="B6" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
@@ -2274,11 +2274,11 @@
       <c r="B15" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
     </row>
     <row r="16" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G16" s="30"/>
@@ -2343,7 +2343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:7" s="15" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" s="15" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="39" t="s">
         <v>67</v>
       </c>
@@ -2388,11 +2388,11 @@
       <c r="B24" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
     </row>
     <row r="25" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G25" s="30"/>
@@ -2437,7 +2437,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="2:7" s="15" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" s="15" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="39" t="s">
         <v>74</v>
       </c>
@@ -2517,11 +2517,11 @@
       <c r="B33" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
     </row>
     <row r="34" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G34" s="30"/>
@@ -2650,11 +2650,11 @@
       <c r="B42" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="54"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="56"/>
     </row>
     <row r="43" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G43" s="30"/>
@@ -2783,11 +2783,11 @@
       <c r="B51" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="C51" s="54"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="54"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
     </row>
     <row r="52" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G52" s="30"/>
@@ -2916,11 +2916,11 @@
       <c r="B60" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="C60" s="54"/>
-      <c r="D60" s="54"/>
-      <c r="E60" s="54"/>
-      <c r="F60" s="54"/>
-      <c r="G60" s="54"/>
+      <c r="C60" s="56"/>
+      <c r="D60" s="56"/>
+      <c r="E60" s="56"/>
+      <c r="F60" s="56"/>
+      <c r="G60" s="56"/>
     </row>
     <row r="61" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G61" s="30"/>
@@ -3055,11 +3055,11 @@
       <c r="B68" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="C68" s="54"/>
-      <c r="D68" s="54"/>
-      <c r="E68" s="54"/>
-      <c r="F68" s="54"/>
-      <c r="G68" s="54"/>
+      <c r="C68" s="56"/>
+      <c r="D68" s="56"/>
+      <c r="E68" s="56"/>
+      <c r="F68" s="56"/>
+      <c r="G68" s="56"/>
       <c r="H68" s="15"/>
       <c r="I68" s="15"/>
       <c r="J68" s="15"/>
@@ -3210,11 +3210,11 @@
       <c r="B77" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="C77" s="54"/>
-      <c r="D77" s="54"/>
-      <c r="E77" s="54"/>
-      <c r="F77" s="54"/>
-      <c r="G77" s="54"/>
+      <c r="C77" s="56"/>
+      <c r="D77" s="56"/>
+      <c r="E77" s="56"/>
+      <c r="F77" s="56"/>
+      <c r="G77" s="56"/>
       <c r="H77" s="15"/>
       <c r="I77" s="15"/>
       <c r="J77" s="15"/>
@@ -3361,11 +3361,11 @@
       <c r="B85" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="C85" s="54"/>
-      <c r="D85" s="54"/>
-      <c r="E85" s="54"/>
-      <c r="F85" s="54"/>
-      <c r="G85" s="54"/>
+      <c r="C85" s="56"/>
+      <c r="D85" s="56"/>
+      <c r="E85" s="56"/>
+      <c r="F85" s="56"/>
+      <c r="G85" s="56"/>
       <c r="H85" s="15"/>
       <c r="I85" s="15"/>
       <c r="J85" s="15"/>
@@ -3512,11 +3512,11 @@
       <c r="B93" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="C93" s="54"/>
-      <c r="D93" s="54"/>
-      <c r="E93" s="54"/>
-      <c r="F93" s="54"/>
-      <c r="G93" s="54"/>
+      <c r="C93" s="56"/>
+      <c r="D93" s="56"/>
+      <c r="E93" s="56"/>
+      <c r="F93" s="56"/>
+      <c r="G93" s="56"/>
       <c r="H93" s="15"/>
       <c r="I93" s="15"/>
       <c r="J93" s="15"/>
@@ -3788,179 +3788,179 @@
       <c r="K113" s="15"/>
     </row>
     <row r="114" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="53"/>
-      <c r="C114" s="53"/>
-      <c r="D114" s="53"/>
+      <c r="B114" s="54"/>
+      <c r="C114" s="54"/>
+      <c r="D114" s="54"/>
       <c r="E114" s="16"/>
       <c r="F114" s="15"/>
-      <c r="G114" s="53"/>
+      <c r="G114" s="54"/>
       <c r="H114" s="15"/>
       <c r="I114" s="15"/>
       <c r="J114" s="15"/>
       <c r="K114" s="15"/>
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B115" s="53"/>
-      <c r="C115" s="53"/>
-      <c r="D115" s="53"/>
+      <c r="B115" s="54"/>
+      <c r="C115" s="54"/>
+      <c r="D115" s="54"/>
       <c r="E115" s="16"/>
       <c r="F115" s="15"/>
-      <c r="G115" s="53"/>
+      <c r="G115" s="54"/>
       <c r="H115" s="15"/>
       <c r="I115" s="15"/>
       <c r="J115" s="15"/>
       <c r="K115" s="15"/>
     </row>
     <row r="116" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B116" s="53"/>
-      <c r="C116" s="53"/>
-      <c r="D116" s="53"/>
+      <c r="B116" s="54"/>
+      <c r="C116" s="54"/>
+      <c r="D116" s="54"/>
       <c r="E116" s="16"/>
       <c r="F116" s="15"/>
-      <c r="G116" s="53"/>
+      <c r="G116" s="54"/>
       <c r="H116" s="15"/>
       <c r="I116" s="15"/>
       <c r="J116" s="15"/>
       <c r="K116" s="15"/>
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B117" s="53"/>
-      <c r="C117" s="53"/>
-      <c r="D117" s="53"/>
+      <c r="B117" s="54"/>
+      <c r="C117" s="54"/>
+      <c r="D117" s="54"/>
       <c r="E117" s="16"/>
       <c r="F117" s="15"/>
-      <c r="G117" s="53"/>
+      <c r="G117" s="54"/>
       <c r="H117" s="15"/>
       <c r="I117" s="15"/>
       <c r="J117" s="15"/>
       <c r="K117" s="15"/>
     </row>
     <row r="118" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B118" s="53"/>
-      <c r="C118" s="53"/>
-      <c r="D118" s="53"/>
+      <c r="B118" s="54"/>
+      <c r="C118" s="54"/>
+      <c r="D118" s="54"/>
       <c r="E118" s="16"/>
       <c r="F118" s="15"/>
-      <c r="G118" s="53"/>
+      <c r="G118" s="54"/>
       <c r="H118" s="15"/>
       <c r="I118" s="15"/>
       <c r="J118" s="15"/>
       <c r="K118" s="15"/>
     </row>
     <row r="119" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B119" s="53"/>
-      <c r="C119" s="53"/>
-      <c r="D119" s="53"/>
+      <c r="B119" s="54"/>
+      <c r="C119" s="54"/>
+      <c r="D119" s="54"/>
       <c r="E119" s="16"/>
       <c r="F119" s="15"/>
-      <c r="G119" s="53"/>
+      <c r="G119" s="54"/>
       <c r="H119" s="15"/>
       <c r="I119" s="15"/>
       <c r="J119" s="15"/>
       <c r="K119" s="15"/>
     </row>
     <row r="120" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B120" s="53"/>
-      <c r="C120" s="53"/>
-      <c r="D120" s="53"/>
+      <c r="B120" s="54"/>
+      <c r="C120" s="54"/>
+      <c r="D120" s="54"/>
       <c r="E120" s="16"/>
       <c r="F120" s="15"/>
-      <c r="G120" s="53"/>
+      <c r="G120" s="54"/>
       <c r="H120" s="15"/>
       <c r="I120" s="15"/>
       <c r="J120" s="15"/>
       <c r="K120" s="15"/>
     </row>
     <row r="121" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B121" s="53"/>
-      <c r="C121" s="53"/>
-      <c r="D121" s="53"/>
+      <c r="B121" s="54"/>
+      <c r="C121" s="54"/>
+      <c r="D121" s="54"/>
       <c r="E121" s="16"/>
       <c r="F121" s="15"/>
-      <c r="G121" s="53"/>
+      <c r="G121" s="54"/>
       <c r="H121" s="15"/>
       <c r="I121" s="15"/>
       <c r="J121" s="15"/>
       <c r="K121" s="15"/>
     </row>
     <row r="122" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B122" s="53"/>
-      <c r="C122" s="53"/>
-      <c r="D122" s="53"/>
+      <c r="B122" s="54"/>
+      <c r="C122" s="54"/>
+      <c r="D122" s="54"/>
       <c r="E122" s="16"/>
       <c r="F122" s="15"/>
-      <c r="G122" s="53"/>
+      <c r="G122" s="54"/>
       <c r="H122" s="15"/>
       <c r="I122" s="15"/>
       <c r="J122" s="15"/>
       <c r="K122" s="15"/>
     </row>
     <row r="123" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B123" s="53"/>
-      <c r="C123" s="53"/>
-      <c r="D123" s="53"/>
+      <c r="B123" s="54"/>
+      <c r="C123" s="54"/>
+      <c r="D123" s="54"/>
       <c r="E123" s="16"/>
       <c r="F123" s="15"/>
-      <c r="G123" s="53"/>
+      <c r="G123" s="54"/>
       <c r="H123" s="15"/>
       <c r="I123" s="15"/>
       <c r="J123" s="15"/>
       <c r="K123" s="15"/>
     </row>
     <row r="124" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B124" s="53"/>
-      <c r="C124" s="53"/>
-      <c r="D124" s="53"/>
+      <c r="B124" s="54"/>
+      <c r="C124" s="54"/>
+      <c r="D124" s="54"/>
       <c r="E124" s="16"/>
       <c r="F124" s="15"/>
-      <c r="G124" s="53"/>
+      <c r="G124" s="54"/>
       <c r="H124" s="15"/>
       <c r="I124" s="15"/>
       <c r="J124" s="15"/>
       <c r="K124" s="15"/>
     </row>
     <row r="125" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B125" s="53"/>
-      <c r="C125" s="53"/>
-      <c r="D125" s="53"/>
+      <c r="B125" s="54"/>
+      <c r="C125" s="54"/>
+      <c r="D125" s="54"/>
       <c r="E125" s="16"/>
       <c r="F125" s="15"/>
-      <c r="G125" s="53"/>
+      <c r="G125" s="54"/>
       <c r="H125" s="15"/>
       <c r="I125" s="15"/>
       <c r="J125" s="15"/>
       <c r="K125" s="15"/>
     </row>
     <row r="126" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B126" s="53"/>
-      <c r="C126" s="53"/>
-      <c r="D126" s="53"/>
+      <c r="B126" s="54"/>
+      <c r="C126" s="54"/>
+      <c r="D126" s="54"/>
       <c r="E126" s="16"/>
       <c r="F126" s="15"/>
-      <c r="G126" s="53"/>
+      <c r="G126" s="54"/>
       <c r="H126" s="15"/>
       <c r="I126" s="15"/>
       <c r="J126" s="15"/>
       <c r="K126" s="15"/>
     </row>
     <row r="127" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B127" s="53"/>
-      <c r="C127" s="53"/>
-      <c r="D127" s="53"/>
+      <c r="B127" s="54"/>
+      <c r="C127" s="54"/>
+      <c r="D127" s="54"/>
       <c r="E127" s="16"/>
       <c r="F127" s="15"/>
-      <c r="G127" s="53"/>
+      <c r="G127" s="54"/>
       <c r="H127" s="15"/>
       <c r="I127" s="15"/>
       <c r="J127" s="15"/>
       <c r="K127" s="15"/>
     </row>
     <row r="128" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B128" s="58"/>
-      <c r="C128" s="58"/>
-      <c r="D128" s="58"/>
-      <c r="E128" s="58"/>
-      <c r="F128" s="58"/>
+      <c r="B128" s="53"/>
+      <c r="C128" s="53"/>
+      <c r="D128" s="53"/>
+      <c r="E128" s="53"/>
+      <c r="F128" s="53"/>
       <c r="G128" s="19"/>
       <c r="H128" s="19"/>
       <c r="I128" s="19"/>
@@ -4004,383 +4004,383 @@
       <c r="K132" s="20"/>
     </row>
     <row r="133" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B133" s="56"/>
-      <c r="C133" s="53"/>
-      <c r="D133" s="53"/>
+      <c r="B133" s="58"/>
+      <c r="C133" s="54"/>
+      <c r="D133" s="54"/>
       <c r="E133" s="16"/>
       <c r="F133" s="15"/>
-      <c r="G133" s="53"/>
+      <c r="G133" s="54"/>
       <c r="H133" s="15"/>
       <c r="I133" s="15"/>
       <c r="J133" s="15"/>
       <c r="K133" s="15"/>
     </row>
     <row r="134" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B134" s="56"/>
-      <c r="C134" s="53"/>
-      <c r="D134" s="53"/>
+      <c r="B134" s="58"/>
+      <c r="C134" s="54"/>
+      <c r="D134" s="54"/>
       <c r="E134" s="16"/>
       <c r="F134" s="15"/>
-      <c r="G134" s="53"/>
+      <c r="G134" s="54"/>
       <c r="H134" s="15"/>
       <c r="I134" s="15"/>
       <c r="J134" s="15"/>
       <c r="K134" s="15"/>
     </row>
     <row r="135" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B135" s="56"/>
-      <c r="C135" s="53"/>
-      <c r="D135" s="53"/>
+      <c r="B135" s="58"/>
+      <c r="C135" s="54"/>
+      <c r="D135" s="54"/>
       <c r="E135" s="16"/>
       <c r="F135" s="15"/>
-      <c r="G135" s="53"/>
+      <c r="G135" s="54"/>
       <c r="H135" s="15"/>
       <c r="I135" s="15"/>
       <c r="J135" s="15"/>
       <c r="K135" s="15"/>
     </row>
     <row r="136" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B136" s="56"/>
-      <c r="C136" s="53"/>
-      <c r="D136" s="53"/>
+      <c r="B136" s="58"/>
+      <c r="C136" s="54"/>
+      <c r="D136" s="54"/>
       <c r="E136" s="16"/>
       <c r="F136" s="15"/>
-      <c r="G136" s="53"/>
+      <c r="G136" s="54"/>
       <c r="H136" s="15"/>
       <c r="I136" s="15"/>
       <c r="J136" s="15"/>
       <c r="K136" s="15"/>
     </row>
     <row r="137" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="56"/>
-      <c r="C137" s="53"/>
-      <c r="D137" s="53"/>
+      <c r="B137" s="58"/>
+      <c r="C137" s="54"/>
+      <c r="D137" s="54"/>
       <c r="E137" s="16"/>
       <c r="F137" s="15"/>
-      <c r="G137" s="53"/>
+      <c r="G137" s="54"/>
       <c r="H137" s="15"/>
       <c r="I137" s="15"/>
       <c r="J137" s="15"/>
       <c r="K137" s="15"/>
     </row>
     <row r="138" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B138" s="56"/>
-      <c r="C138" s="53"/>
-      <c r="D138" s="53"/>
+      <c r="B138" s="58"/>
+      <c r="C138" s="54"/>
+      <c r="D138" s="54"/>
       <c r="E138" s="16"/>
       <c r="F138" s="15"/>
-      <c r="G138" s="53"/>
+      <c r="G138" s="54"/>
       <c r="H138" s="15"/>
       <c r="I138" s="15"/>
       <c r="J138" s="15"/>
       <c r="K138" s="15"/>
     </row>
     <row r="139" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B139" s="56"/>
-      <c r="C139" s="53"/>
-      <c r="D139" s="53"/>
+      <c r="B139" s="58"/>
+      <c r="C139" s="54"/>
+      <c r="D139" s="54"/>
       <c r="E139" s="16"/>
       <c r="F139" s="15"/>
-      <c r="G139" s="53"/>
+      <c r="G139" s="54"/>
       <c r="H139" s="15"/>
       <c r="I139" s="15"/>
       <c r="J139" s="15"/>
       <c r="K139" s="15"/>
     </row>
     <row r="140" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B140" s="56"/>
-      <c r="C140" s="53"/>
-      <c r="D140" s="53"/>
+      <c r="B140" s="58"/>
+      <c r="C140" s="54"/>
+      <c r="D140" s="54"/>
       <c r="E140" s="16"/>
       <c r="F140" s="15"/>
-      <c r="G140" s="53"/>
+      <c r="G140" s="54"/>
       <c r="H140" s="15"/>
       <c r="I140" s="15"/>
       <c r="J140" s="15"/>
       <c r="K140" s="15"/>
     </row>
     <row r="141" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B141" s="56"/>
-      <c r="C141" s="53"/>
-      <c r="D141" s="53"/>
+      <c r="B141" s="58"/>
+      <c r="C141" s="54"/>
+      <c r="D141" s="54"/>
       <c r="E141" s="16"/>
       <c r="F141" s="15"/>
-      <c r="G141" s="53"/>
+      <c r="G141" s="54"/>
       <c r="H141" s="15"/>
       <c r="I141" s="15"/>
       <c r="J141" s="15"/>
       <c r="K141" s="15"/>
     </row>
     <row r="142" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B142" s="56"/>
-      <c r="C142" s="53"/>
-      <c r="D142" s="53"/>
+      <c r="B142" s="58"/>
+      <c r="C142" s="54"/>
+      <c r="D142" s="54"/>
       <c r="E142" s="16"/>
       <c r="F142" s="15"/>
-      <c r="G142" s="53"/>
+      <c r="G142" s="54"/>
       <c r="H142" s="15"/>
       <c r="I142" s="15"/>
       <c r="J142" s="15"/>
       <c r="K142" s="15"/>
     </row>
     <row r="143" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B143" s="56"/>
-      <c r="C143" s="53"/>
-      <c r="D143" s="53"/>
+      <c r="B143" s="58"/>
+      <c r="C143" s="54"/>
+      <c r="D143" s="54"/>
       <c r="E143" s="16"/>
       <c r="F143" s="15"/>
-      <c r="G143" s="53"/>
+      <c r="G143" s="54"/>
       <c r="H143" s="15"/>
       <c r="I143" s="15"/>
       <c r="J143" s="15"/>
       <c r="K143" s="15"/>
     </row>
     <row r="144" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B144" s="56"/>
-      <c r="C144" s="53"/>
-      <c r="D144" s="53"/>
+      <c r="B144" s="58"/>
+      <c r="C144" s="54"/>
+      <c r="D144" s="54"/>
       <c r="E144" s="16"/>
       <c r="F144" s="15"/>
-      <c r="G144" s="53"/>
+      <c r="G144" s="54"/>
       <c r="H144" s="15"/>
       <c r="I144" s="15"/>
       <c r="J144" s="15"/>
       <c r="K144" s="15"/>
     </row>
     <row r="145" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B145" s="56"/>
-      <c r="C145" s="53"/>
-      <c r="D145" s="53"/>
+      <c r="B145" s="58"/>
+      <c r="C145" s="54"/>
+      <c r="D145" s="54"/>
       <c r="E145" s="16"/>
       <c r="F145" s="15"/>
-      <c r="G145" s="53"/>
+      <c r="G145" s="54"/>
       <c r="H145" s="15"/>
       <c r="I145" s="15"/>
       <c r="J145" s="15"/>
       <c r="K145" s="15"/>
     </row>
     <row r="146" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="53"/>
-      <c r="C146" s="53"/>
-      <c r="D146" s="53"/>
+      <c r="B146" s="54"/>
+      <c r="C146" s="54"/>
+      <c r="D146" s="54"/>
       <c r="E146" s="16"/>
       <c r="F146" s="15"/>
-      <c r="G146" s="53"/>
+      <c r="G146" s="54"/>
       <c r="H146" s="15"/>
       <c r="I146" s="15"/>
       <c r="J146" s="15"/>
       <c r="K146" s="15"/>
     </row>
     <row r="147" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B147" s="53"/>
-      <c r="C147" s="53"/>
-      <c r="D147" s="53"/>
+      <c r="B147" s="54"/>
+      <c r="C147" s="54"/>
+      <c r="D147" s="54"/>
       <c r="E147" s="16"/>
       <c r="F147" s="15"/>
-      <c r="G147" s="53"/>
+      <c r="G147" s="54"/>
       <c r="H147" s="15"/>
       <c r="I147" s="15"/>
       <c r="J147" s="15"/>
       <c r="K147" s="15"/>
     </row>
     <row r="148" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B148" s="53"/>
-      <c r="C148" s="53"/>
-      <c r="D148" s="53"/>
+      <c r="B148" s="54"/>
+      <c r="C148" s="54"/>
+      <c r="D148" s="54"/>
       <c r="E148" s="16"/>
       <c r="F148" s="15"/>
-      <c r="G148" s="53"/>
+      <c r="G148" s="54"/>
       <c r="H148" s="15"/>
       <c r="I148" s="15"/>
       <c r="J148" s="15"/>
       <c r="K148" s="15"/>
     </row>
     <row r="149" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B149" s="53"/>
-      <c r="C149" s="53"/>
-      <c r="D149" s="53"/>
+      <c r="B149" s="54"/>
+      <c r="C149" s="54"/>
+      <c r="D149" s="54"/>
       <c r="E149" s="16"/>
       <c r="F149" s="15"/>
-      <c r="G149" s="53"/>
+      <c r="G149" s="54"/>
       <c r="H149" s="15"/>
       <c r="I149" s="15"/>
       <c r="J149" s="15"/>
       <c r="K149" s="15"/>
     </row>
     <row r="150" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B150" s="53"/>
-      <c r="C150" s="53"/>
-      <c r="D150" s="53"/>
+      <c r="B150" s="54"/>
+      <c r="C150" s="54"/>
+      <c r="D150" s="54"/>
       <c r="E150" s="16"/>
       <c r="F150" s="15"/>
-      <c r="G150" s="53"/>
+      <c r="G150" s="54"/>
       <c r="H150" s="15"/>
       <c r="I150" s="15"/>
       <c r="J150" s="15"/>
       <c r="K150" s="15"/>
     </row>
     <row r="151" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B151" s="53"/>
-      <c r="C151" s="53"/>
-      <c r="D151" s="53"/>
+      <c r="B151" s="54"/>
+      <c r="C151" s="54"/>
+      <c r="D151" s="54"/>
       <c r="E151" s="16"/>
       <c r="F151" s="15"/>
-      <c r="G151" s="53"/>
+      <c r="G151" s="54"/>
       <c r="H151" s="15"/>
       <c r="I151" s="15"/>
       <c r="J151" s="15"/>
       <c r="K151" s="15"/>
     </row>
     <row r="152" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B152" s="53"/>
-      <c r="C152" s="53"/>
-      <c r="D152" s="53"/>
+      <c r="B152" s="54"/>
+      <c r="C152" s="54"/>
+      <c r="D152" s="54"/>
       <c r="E152" s="16"/>
       <c r="F152" s="15"/>
-      <c r="G152" s="53"/>
+      <c r="G152" s="54"/>
       <c r="H152" s="15"/>
       <c r="I152" s="15"/>
       <c r="J152" s="15"/>
       <c r="K152" s="15"/>
     </row>
     <row r="153" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="53"/>
-      <c r="C153" s="53"/>
-      <c r="D153" s="53"/>
+      <c r="B153" s="54"/>
+      <c r="C153" s="54"/>
+      <c r="D153" s="54"/>
       <c r="E153" s="16"/>
       <c r="F153" s="15"/>
-      <c r="G153" s="53"/>
+      <c r="G153" s="54"/>
       <c r="H153" s="15"/>
       <c r="I153" s="15"/>
       <c r="J153" s="15"/>
       <c r="K153" s="15"/>
     </row>
     <row r="154" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B154" s="53"/>
-      <c r="C154" s="53"/>
-      <c r="D154" s="53"/>
+      <c r="B154" s="54"/>
+      <c r="C154" s="54"/>
+      <c r="D154" s="54"/>
       <c r="E154" s="16"/>
       <c r="F154" s="15"/>
-      <c r="G154" s="53"/>
+      <c r="G154" s="54"/>
       <c r="H154" s="15"/>
       <c r="I154" s="15"/>
       <c r="J154" s="15"/>
       <c r="K154" s="15"/>
     </row>
     <row r="155" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B155" s="53"/>
-      <c r="C155" s="53"/>
-      <c r="D155" s="53"/>
+      <c r="B155" s="54"/>
+      <c r="C155" s="54"/>
+      <c r="D155" s="54"/>
       <c r="E155" s="16"/>
       <c r="F155" s="15"/>
-      <c r="G155" s="53"/>
+      <c r="G155" s="54"/>
       <c r="H155" s="15"/>
       <c r="I155" s="15"/>
       <c r="J155" s="15"/>
       <c r="K155" s="15"/>
     </row>
     <row r="156" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B156" s="53"/>
-      <c r="C156" s="53"/>
-      <c r="D156" s="53"/>
+      <c r="B156" s="54"/>
+      <c r="C156" s="54"/>
+      <c r="D156" s="54"/>
       <c r="E156" s="16"/>
       <c r="F156" s="15"/>
-      <c r="G156" s="53"/>
+      <c r="G156" s="54"/>
       <c r="H156" s="15"/>
       <c r="I156" s="15"/>
       <c r="J156" s="15"/>
       <c r="K156" s="15"/>
     </row>
     <row r="157" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="53"/>
-      <c r="C157" s="53"/>
-      <c r="D157" s="53"/>
+      <c r="B157" s="54"/>
+      <c r="C157" s="54"/>
+      <c r="D157" s="54"/>
       <c r="E157" s="16"/>
       <c r="F157" s="15"/>
-      <c r="G157" s="53"/>
+      <c r="G157" s="54"/>
       <c r="H157" s="15"/>
       <c r="I157" s="15"/>
       <c r="J157" s="15"/>
       <c r="K157" s="15"/>
     </row>
     <row r="158" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B158" s="53"/>
-      <c r="C158" s="53"/>
-      <c r="D158" s="53"/>
+      <c r="B158" s="54"/>
+      <c r="C158" s="54"/>
+      <c r="D158" s="54"/>
       <c r="E158" s="16"/>
       <c r="F158" s="15"/>
-      <c r="G158" s="53"/>
+      <c r="G158" s="54"/>
       <c r="H158" s="15"/>
       <c r="I158" s="15"/>
       <c r="J158" s="15"/>
       <c r="K158" s="15"/>
     </row>
     <row r="159" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B159" s="53"/>
-      <c r="C159" s="53"/>
-      <c r="D159" s="53"/>
+      <c r="B159" s="54"/>
+      <c r="C159" s="54"/>
+      <c r="D159" s="54"/>
       <c r="E159" s="16"/>
       <c r="F159" s="15"/>
-      <c r="G159" s="53"/>
+      <c r="G159" s="54"/>
       <c r="H159" s="15"/>
       <c r="I159" s="15"/>
       <c r="J159" s="15"/>
       <c r="K159" s="15"/>
     </row>
     <row r="160" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B160" s="53"/>
-      <c r="C160" s="53"/>
-      <c r="D160" s="53"/>
+      <c r="B160" s="54"/>
+      <c r="C160" s="54"/>
+      <c r="D160" s="54"/>
       <c r="E160" s="16"/>
       <c r="F160" s="15"/>
-      <c r="G160" s="53"/>
+      <c r="G160" s="54"/>
       <c r="H160" s="15"/>
       <c r="I160" s="15"/>
       <c r="J160" s="15"/>
       <c r="K160" s="15"/>
     </row>
     <row r="161" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B161" s="53"/>
-      <c r="C161" s="53"/>
-      <c r="D161" s="53"/>
+      <c r="B161" s="54"/>
+      <c r="C161" s="54"/>
+      <c r="D161" s="54"/>
       <c r="E161" s="16"/>
       <c r="F161" s="15"/>
-      <c r="G161" s="53"/>
+      <c r="G161" s="54"/>
       <c r="H161" s="15"/>
       <c r="I161" s="15"/>
       <c r="J161" s="15"/>
       <c r="K161" s="15"/>
     </row>
     <row r="162" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B162" s="53"/>
-      <c r="C162" s="53"/>
-      <c r="D162" s="53"/>
+      <c r="B162" s="54"/>
+      <c r="C162" s="54"/>
+      <c r="D162" s="54"/>
       <c r="E162" s="16"/>
       <c r="F162" s="15"/>
-      <c r="G162" s="53"/>
+      <c r="G162" s="54"/>
       <c r="H162" s="15"/>
       <c r="I162" s="15"/>
       <c r="J162" s="15"/>
       <c r="K162" s="15"/>
     </row>
     <row r="163" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B163" s="53"/>
-      <c r="C163" s="53"/>
-      <c r="D163" s="53"/>
+      <c r="B163" s="54"/>
+      <c r="C163" s="54"/>
+      <c r="D163" s="54"/>
       <c r="E163" s="16"/>
       <c r="F163" s="15"/>
-      <c r="G163" s="53"/>
+      <c r="G163" s="54"/>
       <c r="H163" s="15"/>
       <c r="I163" s="15"/>
       <c r="J163" s="15"/>
       <c r="K163" s="15"/>
     </row>
     <row r="164" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B164" s="58"/>
-      <c r="C164" s="58"/>
-      <c r="D164" s="58"/>
-      <c r="E164" s="58"/>
-      <c r="F164" s="58"/>
+      <c r="B164" s="53"/>
+      <c r="C164" s="53"/>
+      <c r="D164" s="53"/>
+      <c r="E164" s="53"/>
+      <c r="F164" s="53"/>
       <c r="G164" s="19"/>
       <c r="H164" s="19"/>
       <c r="I164" s="19"/>
@@ -4424,167 +4424,167 @@
       <c r="K169" s="20"/>
     </row>
     <row r="170" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B170" s="56"/>
-      <c r="C170" s="53"/>
-      <c r="D170" s="53"/>
+      <c r="B170" s="58"/>
+      <c r="C170" s="54"/>
+      <c r="D170" s="54"/>
       <c r="E170" s="16"/>
       <c r="F170" s="15"/>
-      <c r="G170" s="53"/>
+      <c r="G170" s="54"/>
       <c r="H170" s="15"/>
       <c r="I170" s="15"/>
       <c r="J170" s="15"/>
       <c r="K170" s="15"/>
     </row>
     <row r="171" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B171" s="56"/>
-      <c r="C171" s="53"/>
-      <c r="D171" s="53"/>
+      <c r="B171" s="58"/>
+      <c r="C171" s="54"/>
+      <c r="D171" s="54"/>
       <c r="E171" s="16"/>
       <c r="F171" s="15"/>
-      <c r="G171" s="53"/>
+      <c r="G171" s="54"/>
       <c r="H171" s="15"/>
       <c r="I171" s="15"/>
       <c r="J171" s="15"/>
       <c r="K171" s="15"/>
     </row>
     <row r="172" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B172" s="56"/>
-      <c r="C172" s="53"/>
-      <c r="D172" s="53"/>
+      <c r="B172" s="58"/>
+      <c r="C172" s="54"/>
+      <c r="D172" s="54"/>
       <c r="E172" s="16"/>
       <c r="F172" s="15"/>
-      <c r="G172" s="53"/>
+      <c r="G172" s="54"/>
       <c r="H172" s="15"/>
       <c r="I172" s="15"/>
       <c r="J172" s="15"/>
       <c r="K172" s="15"/>
     </row>
     <row r="173" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B173" s="56"/>
-      <c r="C173" s="53"/>
-      <c r="D173" s="53"/>
+      <c r="B173" s="58"/>
+      <c r="C173" s="54"/>
+      <c r="D173" s="54"/>
       <c r="E173" s="16"/>
       <c r="F173" s="15"/>
-      <c r="G173" s="53"/>
+      <c r="G173" s="54"/>
       <c r="H173" s="15"/>
       <c r="I173" s="15"/>
       <c r="J173" s="15"/>
       <c r="K173" s="15"/>
     </row>
     <row r="174" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B174" s="56"/>
-      <c r="C174" s="53"/>
-      <c r="D174" s="53"/>
+      <c r="B174" s="58"/>
+      <c r="C174" s="54"/>
+      <c r="D174" s="54"/>
       <c r="E174" s="16"/>
       <c r="F174" s="15"/>
-      <c r="G174" s="53"/>
+      <c r="G174" s="54"/>
       <c r="H174" s="15"/>
       <c r="I174" s="15"/>
       <c r="J174" s="15"/>
       <c r="K174" s="15"/>
     </row>
     <row r="175" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B175" s="56"/>
-      <c r="C175" s="53"/>
-      <c r="D175" s="53"/>
+      <c r="B175" s="58"/>
+      <c r="C175" s="54"/>
+      <c r="D175" s="54"/>
       <c r="E175" s="16"/>
       <c r="F175" s="15"/>
-      <c r="G175" s="53"/>
+      <c r="G175" s="54"/>
       <c r="H175" s="15"/>
       <c r="I175" s="15"/>
       <c r="J175" s="15"/>
       <c r="K175" s="15"/>
     </row>
     <row r="176" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="56"/>
-      <c r="C176" s="53"/>
-      <c r="D176" s="53"/>
+      <c r="B176" s="58"/>
+      <c r="C176" s="54"/>
+      <c r="D176" s="54"/>
       <c r="E176" s="16"/>
       <c r="F176" s="15"/>
-      <c r="G176" s="53"/>
+      <c r="G176" s="54"/>
       <c r="H176" s="15"/>
       <c r="I176" s="15"/>
       <c r="J176" s="15"/>
       <c r="K176" s="15"/>
     </row>
     <row r="177" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B177" s="56"/>
-      <c r="C177" s="53"/>
-      <c r="D177" s="53"/>
+      <c r="B177" s="58"/>
+      <c r="C177" s="54"/>
+      <c r="D177" s="54"/>
       <c r="E177" s="16"/>
       <c r="F177" s="15"/>
-      <c r="G177" s="53"/>
+      <c r="G177" s="54"/>
       <c r="H177" s="15"/>
       <c r="I177" s="15"/>
       <c r="J177" s="15"/>
       <c r="K177" s="15"/>
     </row>
     <row r="178" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B178" s="56"/>
-      <c r="C178" s="53"/>
-      <c r="D178" s="53"/>
+      <c r="B178" s="58"/>
+      <c r="C178" s="54"/>
+      <c r="D178" s="54"/>
       <c r="E178" s="16"/>
       <c r="F178" s="15"/>
-      <c r="G178" s="53"/>
+      <c r="G178" s="54"/>
       <c r="H178" s="15"/>
       <c r="I178" s="15"/>
       <c r="J178" s="15"/>
       <c r="K178" s="15"/>
     </row>
     <row r="179" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B179" s="56"/>
-      <c r="C179" s="53"/>
-      <c r="D179" s="53"/>
+      <c r="B179" s="58"/>
+      <c r="C179" s="54"/>
+      <c r="D179" s="54"/>
       <c r="E179" s="16"/>
       <c r="F179" s="15"/>
-      <c r="G179" s="53"/>
+      <c r="G179" s="54"/>
       <c r="H179" s="15"/>
       <c r="I179" s="15"/>
       <c r="J179" s="15"/>
       <c r="K179" s="15"/>
     </row>
     <row r="180" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B180" s="56"/>
-      <c r="C180" s="53"/>
-      <c r="D180" s="53"/>
+      <c r="B180" s="58"/>
+      <c r="C180" s="54"/>
+      <c r="D180" s="54"/>
       <c r="E180" s="16"/>
       <c r="F180" s="15"/>
-      <c r="G180" s="53"/>
+      <c r="G180" s="54"/>
       <c r="H180" s="15"/>
       <c r="I180" s="15"/>
       <c r="J180" s="15"/>
       <c r="K180" s="15"/>
     </row>
     <row r="181" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B181" s="56"/>
-      <c r="C181" s="53"/>
-      <c r="D181" s="53"/>
+      <c r="B181" s="58"/>
+      <c r="C181" s="54"/>
+      <c r="D181" s="54"/>
       <c r="E181" s="16"/>
       <c r="F181" s="15"/>
-      <c r="G181" s="53"/>
+      <c r="G181" s="54"/>
       <c r="H181" s="15"/>
       <c r="I181" s="15"/>
       <c r="J181" s="15"/>
       <c r="K181" s="15"/>
     </row>
     <row r="182" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B182" s="56"/>
-      <c r="C182" s="53"/>
-      <c r="D182" s="53"/>
+      <c r="B182" s="58"/>
+      <c r="C182" s="54"/>
+      <c r="D182" s="54"/>
       <c r="E182" s="16"/>
       <c r="F182" s="15"/>
-      <c r="G182" s="53"/>
+      <c r="G182" s="54"/>
       <c r="H182" s="15"/>
       <c r="I182" s="15"/>
       <c r="J182" s="15"/>
       <c r="K182" s="15"/>
     </row>
     <row r="183" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B183" s="58"/>
-      <c r="C183" s="58"/>
-      <c r="D183" s="58"/>
-      <c r="E183" s="58"/>
-      <c r="F183" s="58"/>
+      <c r="B183" s="53"/>
+      <c r="C183" s="53"/>
+      <c r="D183" s="53"/>
+      <c r="E183" s="53"/>
+      <c r="F183" s="53"/>
       <c r="G183" s="19"/>
       <c r="H183" s="19"/>
       <c r="I183" s="19"/>
@@ -4760,95 +4760,95 @@
       <c r="K200" s="15"/>
     </row>
     <row r="201" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B201" s="56"/>
-      <c r="C201" s="53"/>
+      <c r="B201" s="58"/>
+      <c r="C201" s="54"/>
       <c r="D201" s="16"/>
       <c r="E201" s="16"/>
       <c r="F201" s="15"/>
-      <c r="G201" s="53"/>
+      <c r="G201" s="54"/>
       <c r="H201" s="15"/>
       <c r="I201" s="15"/>
       <c r="J201" s="15"/>
       <c r="K201" s="15"/>
     </row>
     <row r="202" spans="2:11" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B202" s="56"/>
-      <c r="C202" s="53"/>
-      <c r="D202" s="53"/>
+      <c r="B202" s="58"/>
+      <c r="C202" s="54"/>
+      <c r="D202" s="54"/>
       <c r="E202" s="16"/>
       <c r="F202" s="15"/>
-      <c r="G202" s="53"/>
+      <c r="G202" s="54"/>
       <c r="H202" s="15"/>
       <c r="I202" s="15"/>
       <c r="J202" s="15"/>
       <c r="K202" s="15"/>
     </row>
     <row r="203" spans="2:11" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B203" s="56"/>
-      <c r="C203" s="53"/>
-      <c r="D203" s="53"/>
+      <c r="B203" s="58"/>
+      <c r="C203" s="54"/>
+      <c r="D203" s="54"/>
       <c r="E203" s="16"/>
       <c r="F203" s="15"/>
-      <c r="G203" s="53"/>
+      <c r="G203" s="54"/>
       <c r="H203" s="15"/>
       <c r="I203" s="15"/>
       <c r="J203" s="15"/>
       <c r="K203" s="15"/>
     </row>
     <row r="204" spans="2:11" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B204" s="56"/>
-      <c r="C204" s="53"/>
-      <c r="D204" s="53"/>
+      <c r="B204" s="58"/>
+      <c r="C204" s="54"/>
+      <c r="D204" s="54"/>
       <c r="E204" s="16"/>
       <c r="F204" s="15"/>
-      <c r="G204" s="53"/>
+      <c r="G204" s="54"/>
       <c r="H204" s="15"/>
       <c r="I204" s="15"/>
       <c r="J204" s="15"/>
       <c r="K204" s="15"/>
     </row>
     <row r="205" spans="2:11" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B205" s="56"/>
-      <c r="C205" s="53"/>
+      <c r="B205" s="58"/>
+      <c r="C205" s="54"/>
       <c r="D205" s="16"/>
       <c r="E205" s="16"/>
       <c r="F205" s="15"/>
-      <c r="G205" s="53"/>
+      <c r="G205" s="54"/>
       <c r="H205" s="15"/>
       <c r="I205" s="15"/>
       <c r="J205" s="15"/>
       <c r="K205" s="15"/>
     </row>
     <row r="206" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B206" s="56"/>
-      <c r="C206" s="53"/>
+      <c r="B206" s="58"/>
+      <c r="C206" s="54"/>
       <c r="D206" s="16"/>
       <c r="E206" s="16"/>
       <c r="F206" s="15"/>
-      <c r="G206" s="53"/>
+      <c r="G206" s="54"/>
       <c r="H206" s="15"/>
       <c r="I206" s="15"/>
       <c r="J206" s="15"/>
       <c r="K206" s="15"/>
     </row>
     <row r="207" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B207" s="56"/>
-      <c r="C207" s="53"/>
+      <c r="B207" s="58"/>
+      <c r="C207" s="54"/>
       <c r="D207" s="23"/>
       <c r="E207" s="16"/>
       <c r="F207" s="15"/>
-      <c r="G207" s="53"/>
+      <c r="G207" s="54"/>
       <c r="H207" s="15"/>
       <c r="I207" s="15"/>
       <c r="J207" s="15"/>
       <c r="K207" s="15"/>
     </row>
     <row r="208" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B208" s="58"/>
-      <c r="C208" s="58"/>
-      <c r="D208" s="58"/>
-      <c r="E208" s="58"/>
-      <c r="F208" s="58"/>
+      <c r="B208" s="53"/>
+      <c r="C208" s="53"/>
+      <c r="D208" s="53"/>
+      <c r="E208" s="53"/>
+      <c r="F208" s="53"/>
       <c r="G208" s="19"/>
       <c r="H208" s="19"/>
       <c r="I208" s="19"/>
@@ -4892,71 +4892,71 @@
       <c r="K213" s="20"/>
     </row>
     <row r="214" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B214" s="53"/>
-      <c r="C214" s="53"/>
+      <c r="B214" s="54"/>
+      <c r="C214" s="54"/>
       <c r="D214" s="16"/>
       <c r="E214" s="16"/>
       <c r="F214" s="15"/>
-      <c r="G214" s="53"/>
+      <c r="G214" s="54"/>
       <c r="H214" s="15"/>
       <c r="I214" s="15"/>
       <c r="J214" s="15"/>
       <c r="K214" s="15"/>
     </row>
     <row r="215" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B215" s="53"/>
-      <c r="C215" s="53"/>
+      <c r="B215" s="54"/>
+      <c r="C215" s="54"/>
       <c r="D215" s="16"/>
       <c r="E215" s="16"/>
       <c r="F215" s="15"/>
-      <c r="G215" s="53"/>
+      <c r="G215" s="54"/>
       <c r="H215" s="15"/>
       <c r="I215" s="15"/>
       <c r="J215" s="15"/>
       <c r="K215" s="15"/>
     </row>
     <row r="216" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B216" s="53"/>
-      <c r="C216" s="53"/>
+      <c r="B216" s="54"/>
+      <c r="C216" s="54"/>
       <c r="D216" s="16"/>
       <c r="E216" s="16"/>
       <c r="F216" s="15"/>
-      <c r="G216" s="53"/>
+      <c r="G216" s="54"/>
       <c r="H216" s="15"/>
       <c r="I216" s="15"/>
       <c r="J216" s="15"/>
       <c r="K216" s="15"/>
     </row>
     <row r="217" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B217" s="53"/>
-      <c r="C217" s="53"/>
+      <c r="B217" s="54"/>
+      <c r="C217" s="54"/>
       <c r="D217" s="16"/>
       <c r="E217" s="16"/>
       <c r="F217" s="15"/>
-      <c r="G217" s="53"/>
+      <c r="G217" s="54"/>
       <c r="H217" s="15"/>
       <c r="I217" s="15"/>
       <c r="J217" s="15"/>
       <c r="K217" s="15"/>
     </row>
     <row r="218" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B218" s="53"/>
-      <c r="C218" s="53"/>
+      <c r="B218" s="54"/>
+      <c r="C218" s="54"/>
       <c r="D218" s="16"/>
       <c r="E218" s="16"/>
       <c r="F218" s="15"/>
-      <c r="G218" s="53"/>
+      <c r="G218" s="54"/>
       <c r="H218" s="15"/>
       <c r="I218" s="15"/>
       <c r="J218" s="15"/>
       <c r="K218" s="15"/>
     </row>
     <row r="219" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B219" s="58"/>
-      <c r="C219" s="58"/>
-      <c r="D219" s="58"/>
-      <c r="E219" s="58"/>
-      <c r="F219" s="58"/>
+      <c r="B219" s="53"/>
+      <c r="C219" s="53"/>
+      <c r="D219" s="53"/>
+      <c r="E219" s="53"/>
+      <c r="F219" s="53"/>
       <c r="G219" s="19"/>
       <c r="H219" s="19"/>
       <c r="I219" s="19"/>
@@ -4988,155 +4988,155 @@
       <c r="K224" s="20"/>
     </row>
     <row r="225" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B225" s="53"/>
-      <c r="C225" s="53"/>
+      <c r="B225" s="54"/>
+      <c r="C225" s="54"/>
       <c r="D225" s="16"/>
       <c r="E225" s="16"/>
       <c r="F225" s="15"/>
-      <c r="G225" s="53"/>
+      <c r="G225" s="54"/>
       <c r="H225" s="15"/>
       <c r="I225" s="15"/>
       <c r="J225" s="15"/>
       <c r="K225" s="15"/>
     </row>
     <row r="226" spans="2:25" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B226" s="53"/>
-      <c r="C226" s="53"/>
+      <c r="B226" s="54"/>
+      <c r="C226" s="54"/>
       <c r="D226" s="16"/>
       <c r="E226" s="16"/>
       <c r="F226" s="15"/>
-      <c r="G226" s="53"/>
+      <c r="G226" s="54"/>
       <c r="H226" s="15"/>
       <c r="I226" s="15"/>
       <c r="J226" s="15"/>
       <c r="K226" s="15"/>
     </row>
     <row r="227" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B227" s="53"/>
-      <c r="C227" s="53"/>
+      <c r="B227" s="54"/>
+      <c r="C227" s="54"/>
       <c r="D227" s="16"/>
       <c r="E227" s="16"/>
       <c r="F227" s="15"/>
-      <c r="G227" s="53"/>
+      <c r="G227" s="54"/>
       <c r="H227" s="15"/>
       <c r="I227" s="15"/>
       <c r="J227" s="15"/>
       <c r="K227" s="15"/>
-      <c r="P227" s="56"/>
-      <c r="Q227" s="53"/>
-      <c r="R227" s="53"/>
+      <c r="P227" s="58"/>
+      <c r="Q227" s="54"/>
+      <c r="R227" s="54"/>
       <c r="T227" s="15"/>
-      <c r="U227" s="53"/>
+      <c r="U227" s="54"/>
       <c r="V227" s="15"/>
       <c r="W227" s="15"/>
       <c r="X227" s="15"/>
       <c r="Y227" s="15"/>
     </row>
     <row r="228" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B228" s="53"/>
-      <c r="C228" s="53"/>
+      <c r="B228" s="54"/>
+      <c r="C228" s="54"/>
       <c r="D228" s="16"/>
       <c r="E228" s="16"/>
       <c r="F228" s="15"/>
-      <c r="G228" s="53"/>
+      <c r="G228" s="54"/>
       <c r="H228" s="15"/>
       <c r="I228" s="15"/>
       <c r="J228" s="15"/>
       <c r="K228" s="15"/>
-      <c r="P228" s="56"/>
-      <c r="Q228" s="53"/>
-      <c r="R228" s="53"/>
+      <c r="P228" s="58"/>
+      <c r="Q228" s="54"/>
+      <c r="R228" s="54"/>
       <c r="T228" s="15"/>
-      <c r="U228" s="53"/>
+      <c r="U228" s="54"/>
       <c r="V228" s="15"/>
       <c r="W228" s="15"/>
       <c r="X228" s="15"/>
       <c r="Y228" s="15"/>
     </row>
     <row r="229" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B229" s="53"/>
-      <c r="C229" s="53"/>
+      <c r="B229" s="54"/>
+      <c r="C229" s="54"/>
       <c r="D229" s="16"/>
       <c r="E229" s="16"/>
       <c r="F229" s="15"/>
-      <c r="G229" s="53"/>
+      <c r="G229" s="54"/>
       <c r="H229" s="15"/>
       <c r="I229" s="15"/>
       <c r="J229" s="15"/>
       <c r="K229" s="15"/>
-      <c r="P229" s="56"/>
-      <c r="Q229" s="53"/>
-      <c r="R229" s="53"/>
+      <c r="P229" s="58"/>
+      <c r="Q229" s="54"/>
+      <c r="R229" s="54"/>
       <c r="T229" s="15"/>
-      <c r="U229" s="53"/>
+      <c r="U229" s="54"/>
       <c r="V229" s="15"/>
       <c r="W229" s="15"/>
       <c r="X229" s="15"/>
       <c r="Y229" s="15"/>
     </row>
     <row r="230" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B230" s="53"/>
-      <c r="C230" s="53"/>
+      <c r="B230" s="54"/>
+      <c r="C230" s="54"/>
       <c r="D230" s="16"/>
       <c r="E230" s="16"/>
       <c r="F230" s="15"/>
-      <c r="G230" s="53"/>
+      <c r="G230" s="54"/>
       <c r="H230" s="15"/>
       <c r="I230" s="15"/>
       <c r="J230" s="15"/>
       <c r="K230" s="15"/>
-      <c r="P230" s="56"/>
-      <c r="Q230" s="53"/>
-      <c r="R230" s="53"/>
+      <c r="P230" s="58"/>
+      <c r="Q230" s="54"/>
+      <c r="R230" s="54"/>
       <c r="S230" s="16"/>
       <c r="T230" s="15"/>
-      <c r="U230" s="53"/>
+      <c r="U230" s="54"/>
       <c r="V230" s="15"/>
       <c r="W230" s="15"/>
       <c r="X230" s="15"/>
       <c r="Y230" s="15"/>
     </row>
     <row r="231" spans="2:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B231" s="58"/>
-      <c r="C231" s="58"/>
-      <c r="D231" s="58"/>
-      <c r="E231" s="58"/>
-      <c r="F231" s="58"/>
+      <c r="B231" s="53"/>
+      <c r="C231" s="53"/>
+      <c r="D231" s="53"/>
+      <c r="E231" s="53"/>
+      <c r="F231" s="53"/>
       <c r="G231" s="19"/>
       <c r="H231" s="19"/>
       <c r="I231" s="19"/>
       <c r="J231" s="19"/>
       <c r="K231" s="21"/>
       <c r="L231" s="22"/>
-      <c r="P231" s="56"/>
-      <c r="Q231" s="53"/>
-      <c r="R231" s="53"/>
+      <c r="P231" s="58"/>
+      <c r="Q231" s="54"/>
+      <c r="R231" s="54"/>
       <c r="T231" s="15"/>
-      <c r="U231" s="53"/>
+      <c r="U231" s="54"/>
       <c r="V231" s="15"/>
       <c r="W231" s="15"/>
       <c r="X231" s="15"/>
       <c r="Y231" s="15"/>
     </row>
     <row r="232" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="P232" s="56"/>
-      <c r="Q232" s="53"/>
-      <c r="R232" s="53"/>
+      <c r="P232" s="58"/>
+      <c r="Q232" s="54"/>
+      <c r="R232" s="54"/>
       <c r="S232" s="16"/>
       <c r="T232" s="15"/>
-      <c r="U232" s="53"/>
+      <c r="U232" s="54"/>
       <c r="V232" s="15"/>
       <c r="W232" s="15"/>
       <c r="X232" s="15"/>
       <c r="Y232" s="15"/>
     </row>
     <row r="233" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="P233" s="56"/>
-      <c r="Q233" s="53"/>
-      <c r="R233" s="53"/>
+      <c r="P233" s="58"/>
+      <c r="Q233" s="54"/>
+      <c r="R233" s="54"/>
       <c r="S233" s="16"/>
       <c r="T233" s="15"/>
-      <c r="U233" s="53"/>
+      <c r="U233" s="54"/>
       <c r="V233" s="15"/>
       <c r="W233" s="15"/>
       <c r="X233" s="15"/>
@@ -5153,12 +5153,12 @@
       <c r="I234" s="57"/>
       <c r="J234" s="57"/>
       <c r="K234" s="57"/>
-      <c r="P234" s="56"/>
-      <c r="Q234" s="53"/>
-      <c r="R234" s="53"/>
+      <c r="P234" s="58"/>
+      <c r="Q234" s="54"/>
+      <c r="R234" s="54"/>
       <c r="S234" s="16"/>
       <c r="T234" s="15"/>
-      <c r="U234" s="53"/>
+      <c r="U234" s="54"/>
       <c r="V234" s="15"/>
       <c r="W234" s="15"/>
       <c r="X234" s="15"/>
@@ -5175,12 +5175,12 @@
       <c r="I235" s="15"/>
       <c r="J235" s="15"/>
       <c r="K235" s="15"/>
-      <c r="P235" s="56"/>
-      <c r="Q235" s="53"/>
-      <c r="R235" s="53"/>
+      <c r="P235" s="58"/>
+      <c r="Q235" s="54"/>
+      <c r="R235" s="54"/>
       <c r="S235" s="16"/>
       <c r="T235" s="15"/>
-      <c r="U235" s="53"/>
+      <c r="U235" s="54"/>
       <c r="V235" s="15"/>
       <c r="W235" s="15"/>
       <c r="X235" s="15"/>
@@ -5197,115 +5197,115 @@
       <c r="I236" s="20"/>
       <c r="J236" s="20"/>
       <c r="K236" s="20"/>
-      <c r="P236" s="56"/>
-      <c r="Q236" s="53"/>
-      <c r="R236" s="53"/>
+      <c r="P236" s="58"/>
+      <c r="Q236" s="54"/>
+      <c r="R236" s="54"/>
       <c r="S236" s="16"/>
       <c r="T236" s="15"/>
-      <c r="U236" s="53"/>
+      <c r="U236" s="54"/>
       <c r="V236" s="15"/>
       <c r="W236" s="15"/>
       <c r="X236" s="15"/>
       <c r="Y236" s="15"/>
     </row>
     <row r="237" spans="2:25" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B237" s="53"/>
-      <c r="C237" s="53"/>
+      <c r="B237" s="54"/>
+      <c r="C237" s="54"/>
       <c r="D237" s="16"/>
       <c r="E237" s="16"/>
       <c r="F237" s="15"/>
-      <c r="G237" s="53"/>
+      <c r="G237" s="54"/>
       <c r="H237" s="15"/>
       <c r="I237" s="15"/>
       <c r="J237" s="15"/>
       <c r="K237" s="15"/>
-      <c r="P237" s="56"/>
-      <c r="Q237" s="53"/>
-      <c r="R237" s="53"/>
+      <c r="P237" s="58"/>
+      <c r="Q237" s="54"/>
+      <c r="R237" s="54"/>
       <c r="S237" s="16"/>
       <c r="T237" s="15"/>
-      <c r="U237" s="53"/>
+      <c r="U237" s="54"/>
       <c r="V237" s="15"/>
       <c r="W237" s="15"/>
       <c r="X237" s="15"/>
       <c r="Y237" s="15"/>
     </row>
     <row r="238" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B238" s="53"/>
-      <c r="C238" s="53"/>
+      <c r="B238" s="54"/>
+      <c r="C238" s="54"/>
       <c r="D238" s="16"/>
       <c r="E238" s="16"/>
       <c r="F238" s="15"/>
-      <c r="G238" s="53"/>
+      <c r="G238" s="54"/>
       <c r="H238" s="15"/>
       <c r="I238" s="15"/>
       <c r="J238" s="15"/>
       <c r="K238" s="15"/>
-      <c r="P238" s="56"/>
-      <c r="Q238" s="53"/>
-      <c r="R238" s="53"/>
+      <c r="P238" s="58"/>
+      <c r="Q238" s="54"/>
+      <c r="R238" s="54"/>
       <c r="S238" s="16"/>
       <c r="T238" s="15"/>
-      <c r="U238" s="53"/>
+      <c r="U238" s="54"/>
       <c r="V238" s="15"/>
       <c r="W238" s="15"/>
       <c r="X238" s="15"/>
       <c r="Y238" s="15"/>
     </row>
     <row r="239" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B239" s="53"/>
-      <c r="C239" s="53"/>
+      <c r="B239" s="54"/>
+      <c r="C239" s="54"/>
       <c r="D239" s="16"/>
       <c r="E239" s="16"/>
       <c r="F239" s="15"/>
-      <c r="G239" s="53"/>
+      <c r="G239" s="54"/>
       <c r="H239" s="15"/>
       <c r="I239" s="15"/>
       <c r="J239" s="15"/>
       <c r="K239" s="15"/>
     </row>
     <row r="240" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B240" s="53"/>
-      <c r="C240" s="53"/>
+      <c r="B240" s="54"/>
+      <c r="C240" s="54"/>
       <c r="D240" s="16"/>
       <c r="E240" s="16"/>
       <c r="F240" s="15"/>
-      <c r="G240" s="53"/>
+      <c r="G240" s="54"/>
       <c r="H240" s="15"/>
       <c r="I240" s="15"/>
       <c r="J240" s="15"/>
       <c r="K240" s="15"/>
     </row>
     <row r="241" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B241" s="53"/>
-      <c r="C241" s="53"/>
+      <c r="B241" s="54"/>
+      <c r="C241" s="54"/>
       <c r="D241" s="16"/>
       <c r="E241" s="16"/>
       <c r="F241" s="15"/>
-      <c r="G241" s="53"/>
+      <c r="G241" s="54"/>
       <c r="H241" s="15"/>
       <c r="I241" s="15"/>
       <c r="J241" s="15"/>
       <c r="K241" s="15"/>
     </row>
     <row r="242" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B242" s="53"/>
-      <c r="C242" s="53"/>
+      <c r="B242" s="54"/>
+      <c r="C242" s="54"/>
       <c r="D242" s="16"/>
       <c r="E242" s="16"/>
       <c r="F242" s="15"/>
-      <c r="G242" s="53"/>
+      <c r="G242" s="54"/>
       <c r="H242" s="15"/>
       <c r="I242" s="15"/>
       <c r="J242" s="15"/>
       <c r="K242" s="15"/>
     </row>
     <row r="243" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B243" s="58"/>
-      <c r="C243" s="58"/>
-      <c r="D243" s="58"/>
-      <c r="E243" s="58"/>
-      <c r="F243" s="58"/>
+      <c r="B243" s="53"/>
+      <c r="C243" s="53"/>
+      <c r="D243" s="53"/>
+      <c r="E243" s="53"/>
+      <c r="F243" s="53"/>
       <c r="G243" s="19"/>
       <c r="H243" s="19"/>
       <c r="I243" s="19"/>
@@ -5349,83 +5349,83 @@
       <c r="K248" s="20"/>
     </row>
     <row r="249" spans="2:11" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B249" s="53"/>
-      <c r="C249" s="53"/>
-      <c r="D249" s="53"/>
+      <c r="B249" s="54"/>
+      <c r="C249" s="54"/>
+      <c r="D249" s="54"/>
       <c r="E249" s="16"/>
       <c r="F249" s="15"/>
-      <c r="G249" s="53"/>
+      <c r="G249" s="54"/>
       <c r="H249" s="15"/>
       <c r="I249" s="15"/>
       <c r="J249" s="15"/>
       <c r="K249" s="15"/>
     </row>
     <row r="250" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B250" s="53"/>
-      <c r="C250" s="53"/>
-      <c r="D250" s="53"/>
+      <c r="B250" s="54"/>
+      <c r="C250" s="54"/>
+      <c r="D250" s="54"/>
       <c r="E250" s="16"/>
       <c r="F250" s="15"/>
-      <c r="G250" s="53"/>
+      <c r="G250" s="54"/>
       <c r="H250" s="15"/>
       <c r="I250" s="15"/>
       <c r="J250" s="15"/>
       <c r="K250" s="15"/>
     </row>
     <row r="251" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B251" s="53"/>
-      <c r="C251" s="53"/>
-      <c r="D251" s="53"/>
+      <c r="B251" s="54"/>
+      <c r="C251" s="54"/>
+      <c r="D251" s="54"/>
       <c r="E251" s="16"/>
       <c r="F251" s="15"/>
-      <c r="G251" s="53"/>
+      <c r="G251" s="54"/>
       <c r="H251" s="15"/>
       <c r="I251" s="15"/>
       <c r="J251" s="15"/>
       <c r="K251" s="15"/>
     </row>
     <row r="252" spans="2:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B252" s="53"/>
-      <c r="C252" s="53"/>
+      <c r="B252" s="54"/>
+      <c r="C252" s="54"/>
       <c r="D252" s="16"/>
       <c r="E252" s="16"/>
       <c r="F252" s="15"/>
-      <c r="G252" s="53"/>
+      <c r="G252" s="54"/>
       <c r="H252" s="15"/>
       <c r="I252" s="15"/>
       <c r="J252" s="15"/>
       <c r="K252" s="15"/>
     </row>
     <row r="253" spans="2:11" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B253" s="53"/>
-      <c r="C253" s="53"/>
-      <c r="D253" s="53"/>
+      <c r="B253" s="54"/>
+      <c r="C253" s="54"/>
+      <c r="D253" s="54"/>
       <c r="E253" s="16"/>
       <c r="F253" s="15"/>
-      <c r="G253" s="53"/>
+      <c r="G253" s="54"/>
       <c r="H253" s="15"/>
       <c r="I253" s="15"/>
       <c r="J253" s="15"/>
       <c r="K253" s="15"/>
     </row>
     <row r="254" spans="2:11" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B254" s="53"/>
-      <c r="C254" s="53"/>
-      <c r="D254" s="53"/>
+      <c r="B254" s="54"/>
+      <c r="C254" s="54"/>
+      <c r="D254" s="54"/>
       <c r="E254" s="16"/>
       <c r="F254" s="15"/>
-      <c r="G254" s="53"/>
+      <c r="G254" s="54"/>
       <c r="H254" s="15"/>
       <c r="I254" s="15"/>
       <c r="J254" s="15"/>
       <c r="K254" s="15"/>
     </row>
     <row r="255" spans="2:11" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B255" s="58"/>
-      <c r="C255" s="58"/>
-      <c r="D255" s="58"/>
-      <c r="E255" s="58"/>
-      <c r="F255" s="58"/>
+      <c r="B255" s="53"/>
+      <c r="C255" s="53"/>
+      <c r="D255" s="53"/>
+      <c r="E255" s="53"/>
+      <c r="F255" s="53"/>
       <c r="G255" s="19"/>
       <c r="H255" s="19"/>
       <c r="I255" s="19"/>
@@ -5454,6 +5454,78 @@
     </row>
   </sheetData>
   <mergeCells count="88">
+    <mergeCell ref="D161:D163"/>
+    <mergeCell ref="D176:D182"/>
+    <mergeCell ref="B2:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="D114:D120"/>
+    <mergeCell ref="D137:D140"/>
+    <mergeCell ref="D141:D145"/>
+    <mergeCell ref="D121:D124"/>
+    <mergeCell ref="D133:D136"/>
+    <mergeCell ref="D157:D160"/>
+    <mergeCell ref="B157:B163"/>
+    <mergeCell ref="C157:C163"/>
+    <mergeCell ref="G157:G163"/>
+    <mergeCell ref="B153:B156"/>
+    <mergeCell ref="C153:C156"/>
+    <mergeCell ref="D153:D156"/>
+    <mergeCell ref="G153:G156"/>
+    <mergeCell ref="B133:B145"/>
+    <mergeCell ref="C133:C145"/>
+    <mergeCell ref="B146:B152"/>
+    <mergeCell ref="C146:C152"/>
+    <mergeCell ref="G146:G152"/>
+    <mergeCell ref="D146:D149"/>
+    <mergeCell ref="D150:D152"/>
+    <mergeCell ref="U227:U238"/>
+    <mergeCell ref="B201:B207"/>
+    <mergeCell ref="C201:C207"/>
+    <mergeCell ref="G201:G207"/>
+    <mergeCell ref="D202:D204"/>
+    <mergeCell ref="B211:K211"/>
+    <mergeCell ref="B219:F219"/>
+    <mergeCell ref="C214:C218"/>
+    <mergeCell ref="B214:B218"/>
+    <mergeCell ref="P227:P238"/>
+    <mergeCell ref="Q227:Q238"/>
+    <mergeCell ref="G214:G218"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="C237:C242"/>
+    <mergeCell ref="G237:G242"/>
+    <mergeCell ref="B231:F231"/>
+    <mergeCell ref="R227:R230"/>
+    <mergeCell ref="R231:R232"/>
+    <mergeCell ref="R233:R234"/>
+    <mergeCell ref="G114:G120"/>
+    <mergeCell ref="C114:C120"/>
+    <mergeCell ref="B222:K222"/>
+    <mergeCell ref="B225:B230"/>
+    <mergeCell ref="C225:C230"/>
+    <mergeCell ref="B114:B120"/>
+    <mergeCell ref="G121:G127"/>
+    <mergeCell ref="D125:D127"/>
+    <mergeCell ref="B130:K130"/>
+    <mergeCell ref="G133:G145"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B121:B127"/>
+    <mergeCell ref="C121:C127"/>
+    <mergeCell ref="R235:R236"/>
+    <mergeCell ref="R237:R238"/>
+    <mergeCell ref="B234:K234"/>
+    <mergeCell ref="B237:B242"/>
+    <mergeCell ref="B246:K246"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="G225:G230"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B167:K167"/>
+    <mergeCell ref="B186:K186"/>
+    <mergeCell ref="G170:G182"/>
+    <mergeCell ref="D174:D175"/>
+    <mergeCell ref="D170:D173"/>
+    <mergeCell ref="B170:B182"/>
+    <mergeCell ref="C170:C182"/>
     <mergeCell ref="B255:F255"/>
     <mergeCell ref="B249:B254"/>
     <mergeCell ref="C249:C254"/>
@@ -5470,78 +5542,6 @@
     <mergeCell ref="G249:G254"/>
     <mergeCell ref="D249:D251"/>
     <mergeCell ref="D253:D254"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="G225:G230"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B167:K167"/>
-    <mergeCell ref="B186:K186"/>
-    <mergeCell ref="G170:G182"/>
-    <mergeCell ref="D174:D175"/>
-    <mergeCell ref="D170:D173"/>
-    <mergeCell ref="B170:B182"/>
-    <mergeCell ref="C170:C182"/>
-    <mergeCell ref="R235:R236"/>
-    <mergeCell ref="R237:R238"/>
-    <mergeCell ref="B234:K234"/>
-    <mergeCell ref="B237:B242"/>
-    <mergeCell ref="B246:K246"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="R227:R230"/>
-    <mergeCell ref="R231:R232"/>
-    <mergeCell ref="R233:R234"/>
-    <mergeCell ref="G114:G120"/>
-    <mergeCell ref="C114:C120"/>
-    <mergeCell ref="B222:K222"/>
-    <mergeCell ref="B225:B230"/>
-    <mergeCell ref="C225:C230"/>
-    <mergeCell ref="B114:B120"/>
-    <mergeCell ref="G121:G127"/>
-    <mergeCell ref="D125:D127"/>
-    <mergeCell ref="B130:K130"/>
-    <mergeCell ref="G133:G145"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B121:B127"/>
-    <mergeCell ref="C121:C127"/>
-    <mergeCell ref="U227:U238"/>
-    <mergeCell ref="B201:B207"/>
-    <mergeCell ref="C201:C207"/>
-    <mergeCell ref="G201:G207"/>
-    <mergeCell ref="D202:D204"/>
-    <mergeCell ref="B211:K211"/>
-    <mergeCell ref="B219:F219"/>
-    <mergeCell ref="C214:C218"/>
-    <mergeCell ref="B214:B218"/>
-    <mergeCell ref="P227:P238"/>
-    <mergeCell ref="Q227:Q238"/>
-    <mergeCell ref="G214:G218"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="C237:C242"/>
-    <mergeCell ref="G237:G242"/>
-    <mergeCell ref="B231:F231"/>
-    <mergeCell ref="G153:G156"/>
-    <mergeCell ref="B133:B145"/>
-    <mergeCell ref="C133:C145"/>
-    <mergeCell ref="B146:B152"/>
-    <mergeCell ref="C146:C152"/>
-    <mergeCell ref="G146:G152"/>
-    <mergeCell ref="D146:D149"/>
-    <mergeCell ref="D150:D152"/>
-    <mergeCell ref="D161:D163"/>
-    <mergeCell ref="D176:D182"/>
-    <mergeCell ref="B2:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="D114:D120"/>
-    <mergeCell ref="D137:D140"/>
-    <mergeCell ref="D141:D145"/>
-    <mergeCell ref="D121:D124"/>
-    <mergeCell ref="D133:D136"/>
-    <mergeCell ref="D157:D160"/>
-    <mergeCell ref="B157:B163"/>
-    <mergeCell ref="C157:C163"/>
-    <mergeCell ref="G157:G163"/>
-    <mergeCell ref="B153:B156"/>
-    <mergeCell ref="C153:C156"/>
-    <mergeCell ref="D153:D156"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <conditionalFormatting sqref="F9:F11">

</xml_diff>